<commit_message>
hoàn thành phần model và biz cho quản lý account cá nhân
</commit_message>
<xml_diff>
--- a/docs/Sprint 2 - 1003 To 2203/LogTime.xlsx
+++ b/docs/Sprint 2 - 1003 To 2203/LogTime.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OTHER\Project-e\Github\docs\sprint 2 - 1003 To 2203\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OTHER\Project-e\Github\docs\Sprint 2 - 1003 To 2203\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="6165" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ANLT" sheetId="1" r:id="rId1"/>
     <sheet name="QUANGD" sheetId="2" r:id="rId2"/>
     <sheet name="ANHDT" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="33">
   <si>
     <t>Nhận update từ phía A.Hoàng</t>
   </si>
@@ -119,6 +119,12 @@
   </si>
   <si>
     <t>Common Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOME </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DETAILS </t>
   </si>
 </sst>
 </file>
@@ -517,8 +523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -657,6 +663,9 @@
       </c>
       <c r="G6">
         <v>1</v>
+      </c>
+      <c r="K6">
+        <v>3</v>
       </c>
       <c r="L6">
         <v>3</v>
@@ -690,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A12:A13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -831,10 +840,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,6 +917,22 @@
         <v>12</v>
       </c>
     </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>